<commit_message>
Update for complete scenarios running and plotting
</commit_message>
<xml_diff>
--- a/Zetas.xlsx
+++ b/Zetas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1EABDE-E438-4F1D-8B45-8F543DC8B66F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990187E8-8720-41F6-8FE9-69F1E6DDFEB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0E+00"/>
+    <numFmt numFmtId="165" formatCode="0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -281,10 +281,10 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +568,8 @@
   <dimension ref="A1:XFD76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,17 +887,17 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F11" s="11">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="G11" s="10">
-        <v>0.04</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="H11" s="10">
         <v>0.15</v>
       </c>
       <c r="I11" s="10">
-        <f>10^(-10)</f>
-        <v>1E-10</v>
+        <f>3*10^(-10)</f>
+        <v>3E-10</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>15</v>
@@ -920,17 +920,17 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F12" s="11">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G12" s="10">
-        <v>0.04</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="H12" s="10">
         <v>0.15</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" ref="I12:I13" si="0">10^(-10)</f>
-        <v>1E-10</v>
+        <f t="shared" ref="I12:I13" si="0">3*10^(-10)</f>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -950,17 +950,17 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F13" s="11">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="G13" s="10">
-        <v>0.04</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="H13" s="10">
         <v>0.15</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
-        <v>1E-10</v>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -983,13 +983,13 @@
         <v>0.02</v>
       </c>
       <c r="G14" s="12">
-        <v>0.04</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H14" s="12">
         <v>0.15</v>
       </c>
       <c r="I14" s="12">
-        <v>1E-10</v>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1012,13 +1012,13 @@
         <v>0.01</v>
       </c>
       <c r="G15" s="12">
-        <v>0.04</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H15" s="12">
         <v>0.15</v>
       </c>
       <c r="I15" s="12">
-        <v>1E-10</v>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -1041,13 +1041,13 @@
         <v>0.01</v>
       </c>
       <c r="G16" s="12">
-        <v>0.04</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H16" s="12">
         <v>0.15</v>
       </c>
       <c r="I16" s="12">
-        <v>1E-10</v>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F26" s="21">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="G26" s="20">
         <v>2.3E-2</v>
@@ -1337,7 +1337,7 @@
         <v>0.25</v>
       </c>
       <c r="I26" s="48">
-        <v>4.0000000000000002E-9</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -1366,7 +1366,7 @@
         <v>0.25</v>
       </c>
       <c r="I27" s="48">
-        <v>4.0000000000000002E-9</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1395,7 +1395,7 @@
         <v>0.25</v>
       </c>
       <c r="I28" s="51">
-        <v>4.0000000000000002E-9</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1893,16 +1893,16 @@
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="25">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="G47" s="24">
-        <v>0.14799999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="H47" s="24">
         <v>0.2</v>
       </c>
       <c r="I47" s="16">
-        <v>1E-10</v>
+        <v>7.0000000000000004E-11</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>

</xml_diff>

<commit_message>
PHI included as pre-control indicator
</commit_message>
<xml_diff>
--- a/Zetas.xlsx
+++ b/Zetas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990187E8-8720-41F6-8FE9-69F1E6DDFEB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F724254-AC46-43E0-AC7C-EBDD6F6A576F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,8 +568,8 @@
   <dimension ref="A1:XFD76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>